<commit_message>
updated sample salinity for WS
</commit_message>
<xml_diff>
--- a/tests/data/test_airica/storage_test_Sept21.xlsx
+++ b/tests/data/test_airica/storage_test_Sept21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\lab-work\airica\data\LD_storage_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B7241-6A5C-4D4B-BEE1-D33802A2CE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BB86A8-D165-4FAA-BC77-55C95D7A0329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{7741F939-3579-4835-AC9B-056E5DC56150}"/>
   </bookViews>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD63930-A9D0-4326-B92B-8C89864D4982}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27:V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="U2" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V2" s="1">
         <v>-9999</v>
@@ -884,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="U3" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V3" s="1">
         <v>306.60000000000002</v>
@@ -960,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="U4" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V4" s="1">
         <v>308.39999999999998</v>
@@ -1038,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="U5" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V5" s="1">
         <v>308.60000000000002</v>
@@ -1114,7 +1114,7 @@
         <v>2</v>
       </c>
       <c r="U6" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V6" s="1">
         <v>3270.1</v>
@@ -1192,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="U7" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V7" s="1">
         <v>3270.8</v>
@@ -1268,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="U8" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V8" s="1">
         <v>-9999</v>
@@ -1574,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="U12" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V12" s="1">
         <v>3277.8</v>
@@ -1652,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="U13" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V13" s="1">
         <v>3277.2</v>
@@ -1728,7 +1728,7 @@
         <v>2</v>
       </c>
       <c r="U14" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V14" s="1">
         <v>3281.3</v>
@@ -1804,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="U15" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V15" s="1">
         <v>3277.9</v>
@@ -1880,7 +1880,7 @@
         <v>2</v>
       </c>
       <c r="U16" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V16" s="1">
         <v>3280.2</v>
@@ -1956,7 +1956,7 @@
         <v>2</v>
       </c>
       <c r="U17" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V17" s="1">
         <v>3274.2</v>
@@ -2032,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="U18" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V18" s="1">
         <v>3270.5</v>
@@ -2108,7 +2108,7 @@
         <v>2</v>
       </c>
       <c r="U19" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V19" s="1">
         <v>3271.3</v>
@@ -2183,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="U20" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V20" s="1">
         <v>3272.7</v>
@@ -2258,7 +2258,7 @@
         <v>2</v>
       </c>
       <c r="U21" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V21" s="1">
         <v>3272.9</v>

</xml_diff>